<commit_message>
Amend Registry_Record for IR_M1
</commit_message>
<xml_diff>
--- a/source/_static/report/IRM1_sample_r51.xlsx
+++ b/source/_static/report/IRM1_sample_r51.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\COUNTER\Release 5.1\Sample reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3F6BAAD-3015-493B-ABE9-1658B41D6116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75649F0-5074-49DB-B63E-4C25DEAE8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{330CB27F-9017-4613-B683-8A1B2AF1E1B0}"/>
   </bookViews>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Registry_Record</t>
-  </si>
-  <si>
-    <t>https://registry.projectcounter.org/usage-data-host/99999999-9999-9999-9999-999999999999</t>
   </si>
   <si>
     <t>Item</t>
@@ -610,6 +607,9 @@
   <si>
     <t>804</t>
   </si>
+  <si>
+    <t>https://registry.projectcounter.org/platform/99999999-9999-9999-9999-999999999999</t>
+  </si>
 </sst>
 </file>
 
@@ -631,8 +631,9 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -652,15 +653,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1319,7 +1322,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1368,750 +1371,750 @@
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="U15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="V15" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="I17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="U18" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="V18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="I19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="R19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="U19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="U19" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="V19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="V20" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="I21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="S21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="S21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="U21" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="S22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="U22" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="T23" s="1" t="s">
+      <c r="U23" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="V23" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="S24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T24" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="S24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="T24" s="1" t="s">
+      <c r="U24" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="U24" s="1" t="s">
+      <c r="V24" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="I25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="S25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T25" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T25" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="U25" s="1" t="s">
+      <c r="V25" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Miscellaneous wording changes, clarifications and fixes (part 3) (#231)
</commit_message>
<xml_diff>
--- a/source/_static/report/IRM1_sample_r51.xlsx
+++ b/source/_static/report/IRM1_sample_r51.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\COUNTER\Release 5.1\Sample reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3F6BAAD-3015-493B-ABE9-1658B41D6116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75649F0-5074-49DB-B63E-4C25DEAE8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{330CB27F-9017-4613-B683-8A1B2AF1E1B0}"/>
   </bookViews>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Registry_Record</t>
-  </si>
-  <si>
-    <t>https://registry.projectcounter.org/usage-data-host/99999999-9999-9999-9999-999999999999</t>
   </si>
   <si>
     <t>Item</t>
@@ -610,6 +607,9 @@
   <si>
     <t>804</t>
   </si>
+  <si>
+    <t>https://registry.projectcounter.org/platform/99999999-9999-9999-9999-999999999999</t>
+  </si>
 </sst>
 </file>
 
@@ -631,8 +631,9 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -652,15 +653,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1319,7 +1322,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1368,750 +1371,750 @@
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="U15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="V15" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="I17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="U18" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="V18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="I19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="R19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="U19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="U19" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="V19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="V20" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="I21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="S21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="S21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="U21" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="S22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="U22" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="T23" s="1" t="s">
+      <c r="U23" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="V23" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="S24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T24" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="S24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="T24" s="1" t="s">
+      <c r="U24" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="U24" s="1" t="s">
+      <c r="V24" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="I25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="S25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T25" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T25" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="U25" s="1" t="s">
+      <c r="V25" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>